<commit_message>
v3.2 almost excel for pręt done
</commit_message>
<xml_diff>
--- a/Lab 2 - Wahało fizyczne/PomiaryWahadloFizyczne.xlsx
+++ b/Lab 2 - Wahało fizyczne/PomiaryWahadloFizyczne.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>k</t>
   </si>
@@ -194,6 +194,15 @@
   </si>
   <si>
     <t>u(l)</t>
+  </si>
+  <si>
+    <t>[kg]</t>
+  </si>
+  <si>
+    <t>[m]</t>
+  </si>
+  <si>
+    <t>u(io)</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -604,6 +613,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3664,8 +3679,13 @@
       <c r="B30" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
+      <c r="C30" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="19">
+        <f>C3*0.001</f>
+        <v>1E-3</v>
+      </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
@@ -3747,8 +3767,13 @@
       <c r="B31" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
+      <c r="C31" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="19">
+        <f t="shared" ref="D31:D32" si="4">C4*0.001</f>
+        <v>1E-3</v>
+      </c>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
@@ -3830,8 +3855,13 @@
       <c r="B32" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
+      <c r="C32" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="19">
+        <f>C6*0.001</f>
+        <v>1E-3</v>
+      </c>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
@@ -3909,10 +3939,17 @@
       <c r="CA32" s="19"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
+      <c r="A33" s="48">
+        <v>5</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
+      <c r="D33" s="19">
+        <f>SQRT((D30/(B3*0.001))^2+(D32/(B6*0.001))^2+((2*D25)/D24)^2)</f>
+        <v>4.9402833245746269E-3</v>
+      </c>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
@@ -3990,10 +4027,15 @@
       <c r="CA33" s="19"/>
     </row>
     <row r="34" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
+      <c r="D34" s="19">
+        <f>D33*D27</f>
+        <v>3.9935370226518716E-4</v>
+      </c>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
@@ -4071,10 +4113,15 @@
       <c r="CA34" s="19"/>
     </row>
     <row r="35" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
+      <c r="D35" s="19">
+        <f>SQRT(D34^2+(((B6*0.001)^2)*D30)^2+(-2*B6*0.001*B3*0.001*D30)^2)</f>
+        <v>5.4605141025173783E-4</v>
+      </c>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
@@ -4152,7 +4199,7 @@
       <c r="CA35" s="19"/>
     </row>
     <row r="36" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="A36" s="49"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
@@ -33404,8 +33451,9 @@
       <c r="BQ417" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A35"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A12:D12"/>
@@ -33424,8 +33472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v4.4 almost done :3
</commit_message>
<xml_diff>
--- a/Lab 2 - Wahało fizyczne/PomiaryWahadloFizyczne.xlsx
+++ b/Lab 2 - Wahało fizyczne/PomiaryWahadloFizyczne.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>k</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>ta z 6</t>
+  </si>
+  <si>
+    <t>u(wym-gem)</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -589,6 +592,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -628,11 +639,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -939,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,25 +956,27 @@
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:79" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="40"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="44"/>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
       <c r="L1" s="18"/>
@@ -1928,20 +1937,20 @@
       <c r="CA11" s="18"/>
     </row>
     <row r="12" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="40"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="44"/>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
@@ -3164,22 +3173,22 @@
       <c r="CA23" s="18"/>
     </row>
     <row r="24" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="47"/>
       <c r="D24" s="21">
         <f>AVERAGE(D14:D23)</f>
         <v>1.3357500000000002</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
-      <c r="G24" s="41" t="s">
+      <c r="G24" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="47"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="51"/>
       <c r="J24" s="21">
         <f>AVERAGE(J14:J23)</f>
         <v>1.036</v>
@@ -3255,22 +3264,22 @@
       <c r="CA24" s="18"/>
     </row>
     <row r="25" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="46"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="23">
         <f>SQRT((SUM(E14:E23))/(10*9))</f>
         <v>1.9933918609022078E-3</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
-      <c r="G25" s="44" t="s">
+      <c r="G25" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="H25" s="45"/>
-      <c r="I25" s="46"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
       <c r="J25" s="23">
         <f>SQRT((SUM(K14:K23))/(10*9))</f>
         <v>8.9131613047471259E-4</v>
@@ -3704,7 +3713,7 @@
       <c r="CA29" s="18"/>
     </row>
     <row r="30" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="40" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="18" t="s">
@@ -3719,14 +3728,17 @@
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="36" t="s">
+      <c r="G30" s="40" t="s">
         <v>56</v>
       </c>
       <c r="H30" s="34" t="s">
         <v>17</v>
       </c>
       <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
+      <c r="J30" s="18">
+        <f>I3*0.001/SQRT(3)</f>
+        <v>5.773502691896258E-4</v>
+      </c>
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
@@ -3797,8 +3809,8 @@
       <c r="BZ30" s="18"/>
       <c r="CA30" s="18"/>
     </row>
-    <row r="31" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
+    <row r="31" spans="1:79" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="40"/>
       <c r="B31" s="18" t="s">
         <v>57</v>
       </c>
@@ -3811,12 +3823,15 @@
       </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="36"/>
+      <c r="G31" s="40"/>
       <c r="H31" s="34" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
+      <c r="J31" s="33">
+        <f>I4*0.001/SQRT(3)</f>
+        <v>5.7735026918962585E-5</v>
+      </c>
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
@@ -3888,7 +3903,7 @@
       <c r="CA31" s="18"/>
     </row>
     <row r="32" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="18" t="s">
         <v>19</v>
       </c>
@@ -3901,10 +3916,8 @@
       </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="34" t="s">
-        <v>19</v>
-      </c>
+      <c r="G32" s="40"/>
+      <c r="H32" s="34"/>
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
@@ -3978,7 +3991,7 @@
       <c r="CA32" s="18"/>
     </row>
     <row r="33" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A33" s="37">
+      <c r="A33" s="41">
         <v>5</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -3991,14 +4004,17 @@
       </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
-      <c r="G33" s="37">
+      <c r="G33" s="41">
         <v>5</v>
       </c>
       <c r="H33" s="34" t="s">
         <v>27</v>
       </c>
       <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
+      <c r="J33" s="18">
+        <f>SQRT((J30/(H3*0.001))^2+(J31/(H9*0.001))^2+((2*J25)/J24)^2)</f>
+        <v>1.8249833689050125E-3</v>
+      </c>
       <c r="K33" s="18"/>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
@@ -4070,7 +4086,7 @@
       <c r="CA33" s="18"/>
     </row>
     <row r="34" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="18" t="s">
         <v>60</v>
       </c>
@@ -4081,12 +4097,15 @@
       </c>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
-      <c r="G34" s="37"/>
+      <c r="G34" s="41"/>
       <c r="H34" s="34" t="s">
         <v>60</v>
       </c>
       <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
+      <c r="J34" s="33">
+        <f>J33*J27</f>
+        <v>8.7774855868526716E-5</v>
+      </c>
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
@@ -4158,7 +4177,7 @@
       <c r="CA34" s="18"/>
     </row>
     <row r="35" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="18" t="s">
         <v>22</v>
       </c>
@@ -4169,12 +4188,15 @@
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
-      <c r="G35" s="37"/>
+      <c r="G35" s="41"/>
       <c r="H35" s="34" t="s">
         <v>22</v>
       </c>
       <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
+      <c r="J35" s="36">
+        <f>SQRT(J34^2+(((H9*0.001)^2)*J30)^2+(-2*H9*0.001*H3*0.001*J30)^2)</f>
+        <v>2.2620545307414639E-4</v>
+      </c>
       <c r="K35" s="18"/>
       <c r="L35" s="18"/>
       <c r="M35" s="18"/>
@@ -4253,7 +4275,7 @@
         <v>61</v>
       </c>
       <c r="C36" s="34"/>
-      <c r="D36" s="50">
+      <c r="D36" s="37">
         <f>(SQRT((D30/(B3*0.001))^2+(2*(D31/(B4*0.001)))^2)*D29)</f>
         <v>5.4971299329741155E-5</v>
       </c>
@@ -4266,7 +4288,10 @@
         <v>61</v>
       </c>
       <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="J36" s="33">
+        <f>(SQRT(2*((J30/(H3*0.001))^2)+(2*(J31/(H6*0.001)))^2+(2*(J31/(H7*0.001)))^2)*J29)</f>
+        <v>3.3332162852024711E-5</v>
+      </c>
       <c r="K36" s="34"/>
       <c r="L36" s="34"/>
       <c r="M36" s="34"/>
@@ -4351,7 +4376,9 @@
       <c r="G37" s="34">
         <v>7</v>
       </c>
-      <c r="H37" s="34"/>
+      <c r="H37" s="34" t="s">
+        <v>62</v>
+      </c>
       <c r="I37" s="34"/>
       <c r="J37" s="34"/>
       <c r="K37" s="34"/>
@@ -4425,10 +4452,10 @@
       <c r="CA37" s="18"/>
     </row>
     <row r="38" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
       <c r="E38" s="34"/>
       <c r="F38" s="34"/>
       <c r="G38" s="34"/>
@@ -4506,10 +4533,10 @@
       <c r="CA38" s="18"/>
     </row>
     <row r="39" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
       <c r="E39" s="34"/>
       <c r="F39" s="34"/>
       <c r="G39" s="34"/>
@@ -4587,7 +4614,7 @@
       <c r="CA39" s="18"/>
     </row>
     <row r="40" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A40" s="36"/>
+      <c r="A40" s="40"/>
       <c r="B40" s="34"/>
       <c r="C40" s="34"/>
       <c r="D40" s="34"/>
@@ -4668,7 +4695,7 @@
       <c r="CA40" s="18"/>
     </row>
     <row r="41" spans="1:79" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="34"/>
       <c r="C41" s="34"/>
       <c r="D41" s="34"/>
@@ -33516,12 +33543,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:D39"/>
-    <mergeCell ref="G30:G32"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A35"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A12:D12"/>
@@ -33530,6 +33551,12 @@
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:D39"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -33540,8 +33567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33553,20 +33580,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -33977,11 +34004,11 @@
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4" t="s">
         <v>12</v>
@@ -34088,7 +34115,7 @@
       <c r="H20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="54">
         <f>I19*I31</f>
         <v>8.5342967843876071E-5</v>
       </c>
@@ -34109,7 +34136,7 @@
       <c r="H21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="54">
         <f>SQRT((I20)^2+(I30^2*I17)^2+(2*I30*I29*I18)^2)</f>
         <v>8.6045440799331518E-5</v>
       </c>
@@ -34181,7 +34208,7 @@
       <c r="A26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="51">
+      <c r="B26" s="38">
         <f>B25*B32</f>
         <v>5.4296841817973006E-5</v>
       </c>
@@ -34193,7 +34220,7 @@
       <c r="H26" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="52">
+      <c r="I26" s="39">
         <f>I25*I32</f>
         <v>1.4817031716503434E-5</v>
       </c>
@@ -34205,11 +34232,11 @@
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4" t="s">
         <v>12</v>

</xml_diff>